<commit_message>
Update stopp, acb, output
</commit_message>
<xml_diff>
--- a/ATC_Groepen/ATC_groepen.xlsx
+++ b/ATC_Groepen/ATC_groepen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ppcomm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semde\Documents\MedicatieReview\ATC_Groepen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2138987-BAD8-468D-8E88-F1BC4B063E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7D80DE-84E7-4074-BD97-F39FF4E2731F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="638" windowWidth="21585" windowHeight="13762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,24 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="212">
   <si>
     <t>ATC_groep</t>
   </si>
@@ -535,9 +548,6 @@
     <t>OVERIGE NIET-THERAPEUTISCHE MIDDELEN</t>
   </si>
   <si>
-    <t>Jansen_Omschrijving</t>
-  </si>
-  <si>
     <t>Mond</t>
   </si>
   <si>
@@ -614,6 +624,54 @@
   </si>
   <si>
     <t>Anabolen</t>
+  </si>
+  <si>
+    <t>Vaccins</t>
+  </si>
+  <si>
+    <t>Spierrelaxantia</t>
+  </si>
+  <si>
+    <t>Immunosuppressiva</t>
+  </si>
+  <si>
+    <t>Immunostimulantia</t>
+  </si>
+  <si>
+    <t>Hormonen</t>
+  </si>
+  <si>
+    <t>Oncolytica</t>
+  </si>
+  <si>
+    <t>Sera en immunoglobulinen</t>
+  </si>
+  <si>
+    <t>Antimycobacteriele middelen</t>
+  </si>
+  <si>
+    <t>Antivirale middelen</t>
+  </si>
+  <si>
+    <t>Antimycotica</t>
+  </si>
+  <si>
+    <t>Calciumregulerende middelen</t>
+  </si>
+  <si>
+    <t>Pancreashormonen</t>
+  </si>
+  <si>
+    <t>Schildklierhormonen</t>
+  </si>
+  <si>
+    <t>Corticosteroiden systemisch</t>
+  </si>
+  <si>
+    <t>Hypofyse- en hypothalamus en verwante verbindingen</t>
+  </si>
+  <si>
+    <t>Jansen_omschrijving</t>
   </si>
 </sst>
 </file>
@@ -685,7 +743,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -988,18 +1046,18 @@
   <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,10 +1065,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1018,10 +1076,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1029,10 +1087,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1040,10 +1098,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1051,10 +1109,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1062,10 +1120,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1073,10 +1131,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1084,10 +1142,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1095,10 +1153,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1106,10 +1164,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1117,10 +1175,10 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1128,10 +1186,10 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1139,10 +1197,10 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1150,10 +1208,10 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1161,10 +1219,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1172,10 +1230,10 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1183,10 +1241,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1194,10 +1252,10 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1205,10 +1263,10 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1216,10 +1274,10 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1227,10 +1285,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1238,10 +1296,10 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1249,10 +1307,10 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1260,10 +1318,10 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1271,10 +1329,10 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1282,10 +1340,10 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1293,10 +1351,10 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1304,10 +1362,10 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1315,10 +1373,10 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1326,10 +1384,10 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1337,10 +1395,10 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1348,10 +1406,10 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1359,10 +1417,10 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1370,10 +1428,10 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1381,10 +1439,10 @@
         <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1392,10 +1450,10 @@
         <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1403,10 +1461,10 @@
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1414,10 +1472,10 @@
         <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1425,10 +1483,10 @@
         <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1436,10 +1494,10 @@
         <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1447,10 +1505,10 @@
         <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1458,70 +1516,65 @@
         <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>84</v>
       </c>
       <c r="B43" t="s">
         <v>85</v>
       </c>
-      <c r="C43" t="str">
-        <f t="shared" ref="C3:C66" si="0">B43</f>
-        <v>HYPOFYSE- EN HYPOTHALAMUSHORMONEN EN VERWANTE VERBINDINGEN</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>87</v>
       </c>
-      <c r="C44" t="str">
-        <f t="shared" si="0"/>
-        <v>CORTICOSTEROIDEN VOOR SYSTEMISCH GEBRUIK</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>88</v>
       </c>
       <c r="B45" t="s">
         <v>89</v>
       </c>
-      <c r="C45" t="str">
-        <f t="shared" si="0"/>
-        <v>SCHILDKLIERMIDDELEN</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>90</v>
       </c>
       <c r="B46" t="s">
         <v>91</v>
       </c>
-      <c r="C46" t="str">
-        <f t="shared" si="0"/>
-        <v>PANCREASHORMONEN</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>92</v>
       </c>
       <c r="B47" t="s">
         <v>93</v>
       </c>
-      <c r="C47" t="str">
-        <f t="shared" si="0"/>
-        <v>CALCIUMREGULERENDE MIDDELEN</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -1529,118 +1582,109 @@
         <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="C49" t="str">
-        <f t="shared" si="0"/>
-        <v>ANTIMYCOTICA VOOR SYSTEMISCH GEBRUIK</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>98</v>
       </c>
       <c r="B50" t="s">
         <v>99</v>
       </c>
-      <c r="C50" t="str">
-        <f t="shared" si="0"/>
-        <v>ANTIMYCOBACTERIELE MIDDELEN</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>100</v>
       </c>
       <c r="B51" t="s">
         <v>101</v>
       </c>
-      <c r="C51" t="str">
-        <f t="shared" si="0"/>
-        <v>ANTIVIRALE MIDDELEN VOOR SYSTEMISCH GEBRUIK</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>102</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
       </c>
-      <c r="C52" t="str">
-        <f t="shared" si="0"/>
-        <v>SERA EN IMMUNOGLOBULINEN</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>104</v>
       </c>
       <c r="B53" t="s">
         <v>105</v>
       </c>
-      <c r="C53" t="str">
-        <f t="shared" si="0"/>
-        <v>VACCINS</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>106</v>
       </c>
       <c r="B54" t="s">
         <v>107</v>
       </c>
-      <c r="C54" t="str">
-        <f t="shared" si="0"/>
-        <v>ONCOLYTICA</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>108</v>
       </c>
       <c r="B55" t="s">
         <v>109</v>
       </c>
-      <c r="C55" t="str">
-        <f t="shared" si="0"/>
-        <v>HORMONEN</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>110</v>
       </c>
       <c r="B56" t="s">
         <v>111</v>
       </c>
-      <c r="C56" t="str">
-        <f t="shared" si="0"/>
-        <v>IMMUNOSTIMULANTIA</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>112</v>
       </c>
       <c r="B57" t="s">
         <v>113</v>
       </c>
-      <c r="C57" t="str">
-        <f t="shared" si="0"/>
-        <v>IMMUNOSUPPRESSIVA</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -1648,10 +1692,10 @@
         <v>115</v>
       </c>
       <c r="C58" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -1659,22 +1703,21 @@
         <v>117</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>118</v>
       </c>
       <c r="B60" t="s">
         <v>119</v>
       </c>
-      <c r="C60" t="str">
-        <f t="shared" si="0"/>
-        <v>SPIERRELAXANTIA</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -1682,10 +1725,10 @@
         <v>121</v>
       </c>
       <c r="C61" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -1693,10 +1736,10 @@
         <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -1704,10 +1747,10 @@
         <v>125</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -1715,10 +1758,10 @@
         <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -1726,10 +1769,10 @@
         <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -1737,10 +1780,10 @@
         <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -1748,10 +1791,10 @@
         <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -1759,10 +1802,10 @@
         <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -1770,10 +1813,10 @@
         <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -1781,10 +1824,10 @@
         <v>139</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -1792,10 +1835,10 @@
         <v>141</v>
       </c>
       <c r="C71" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -1803,10 +1846,10 @@
         <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -1814,10 +1857,10 @@
         <v>145</v>
       </c>
       <c r="C73" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -1825,10 +1868,10 @@
         <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -1836,10 +1879,10 @@
         <v>149</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -1847,10 +1890,10 @@
         <v>151</v>
       </c>
       <c r="C76" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -1858,10 +1901,10 @@
         <v>153</v>
       </c>
       <c r="C77" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -1869,10 +1912,10 @@
         <v>155</v>
       </c>
       <c r="C78" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -1880,10 +1923,10 @@
         <v>157</v>
       </c>
       <c r="C79" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -1891,10 +1934,10 @@
         <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>160</v>
       </c>
@@ -1902,10 +1945,10 @@
         <v>161</v>
       </c>
       <c r="C81" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -1913,10 +1956,10 @@
         <v>163</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -1924,10 +1967,10 @@
         <v>165</v>
       </c>
       <c r="C83" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -1935,10 +1978,10 @@
         <v>167</v>
       </c>
       <c r="C84" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>168</v>
       </c>
@@ -1946,7 +1989,7 @@
         <v>169</v>
       </c>
       <c r="C85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>